<commit_message>
Data can be used as trend data
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST_lvl2-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST_lvl2-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>iso</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>use_as_trend</t>
+  </si>
+  <si>
+    <t>match_year</t>
   </si>
 </sst>
 </file>
@@ -469,15 +475,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +517,14 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -530,6 +545,12 @@
       </c>
       <c r="J2" t="s">
         <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>1953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User percentage breakdowns can now be specified
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST_lvl2-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST_lvl2-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>iso</t>
   </si>
@@ -82,16 +82,38 @@
   </si>
   <si>
     <t>match_year</t>
+  </si>
+  <si>
+    <t>specified_breakdowns</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,13 +136,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -460,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,7 +497,7 @@
     <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +522,11 @@
       <c r="H1" t="s">
         <v>18</v>
       </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -517,10 +546,13 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>1953</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>